<commit_message>
updated project plan docs
</commit_message>
<xml_diff>
--- a/planning-docs/CST-451_Test_Cases.xlsx
+++ b/planning-docs/CST-451_Test_Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Project Name:</t>
   </si>
@@ -139,7 +139,7 @@
     <t>Test world name: "MyFirstWorld"</t>
   </si>
   <si>
-    <t>World is created and user redirected to the avatar select screen.</t>
+    <t>World is created and user redirected to the world select screen.</t>
   </si>
   <si>
     <t>Create Protected New World</t>
@@ -691,14 +691,14 @@
     <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1237,8 +1237,12 @@
       <c r="E13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="40"/>
+      <c r="F13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="H13" s="33"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
@@ -1257,8 +1261,12 @@
       <c r="E14" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="40"/>
+      <c r="F14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="H14" s="33"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
@@ -1268,7 +1276,7 @@
       <c r="B15" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="39" t="s">
         <v>43</v>
       </c>
       <c r="D15" s="31" t="s">
@@ -1277,8 +1285,8 @@
       <c r="E15" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
       <c r="H15" s="33"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
@@ -1295,8 +1303,8 @@
       <c r="E16" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="33"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
@@ -1315,8 +1323,8 @@
       <c r="E17" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="33"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
@@ -1335,8 +1343,8 @@
       <c r="E18" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
       <c r="H18" s="33"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
@@ -1355,8 +1363,8 @@
       <c r="E19" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
       <c r="H19" s="33"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
@@ -1375,8 +1383,8 @@
       <c r="E20" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="33"/>
     </row>
     <row r="21">

</xml_diff>